<commit_message>
Load latest Python Project 2 Notebooks
Loading the latest notebooks (both Ken and Jey's), along with updated data output.
</commit_message>
<xml_diff>
--- a/624/Projects/project2_python/data/random_forest_predictions_ken.xlsx
+++ b/624/Projects/project2_python/data/random_forest_predictions_ken.xlsx
@@ -648,7 +648,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z2">
-        <v>8.454138000000254</v>
+        <v>8.595525002827767</v>
       </c>
       <c r="AA2">
         <v>0.022</v>
@@ -749,7 +749,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z3">
-        <v>8.367992999999885</v>
+        <v>8.576272584487292</v>
       </c>
       <c r="AA3">
         <v>0.03</v>
@@ -850,7 +850,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z4">
-        <v>8.433785999999694</v>
+        <v>8.539625559731398</v>
       </c>
       <c r="AA4">
         <v>0.046</v>
@@ -945,7 +945,7 @@
         <v>-4</v>
       </c>
       <c r="Z5">
-        <v>8.537653999999874</v>
+        <v>8.455251211616226</v>
       </c>
       <c r="AB5">
         <v>120</v>
@@ -1043,7 +1043,7 @@
         <v>-4</v>
       </c>
       <c r="Z6">
-        <v>8.446134000000404</v>
+        <v>8.590718104473112</v>
       </c>
       <c r="AA6">
         <v>0.082</v>
@@ -1141,7 +1141,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z7">
-        <v>8.410218000000265</v>
+        <v>8.566806245704996</v>
       </c>
       <c r="AA7">
         <v>0.064</v>
@@ -1242,7 +1242,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z8">
-        <v>8.484595866666986</v>
+        <v>8.476431344444938</v>
       </c>
       <c r="AA8">
         <v>0.042</v>
@@ -1334,7 +1334,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z9">
-        <v>8.46398400000046</v>
+        <v>8.520762609524311</v>
       </c>
       <c r="AA9">
         <v>0.096</v>
@@ -1435,7 +1435,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z10">
-        <v>8.512828000000892</v>
+        <v>8.303527964285454</v>
       </c>
       <c r="AA10">
         <v>0.046</v>
@@ -1533,7 +1533,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z11">
-        <v>8.559332000000483</v>
+        <v>8.670502361904514</v>
       </c>
       <c r="AA11">
         <v>0.096</v>
@@ -1628,7 +1628,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z12">
-        <v>8.540575999999531</v>
+        <v>8.628690203440247</v>
       </c>
       <c r="AA12">
         <v>0.066</v>
@@ -1729,7 +1729,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z13">
-        <v>8.548173999999753</v>
+        <v>8.590718104473112</v>
       </c>
       <c r="AA13">
         <v>0.048</v>
@@ -1830,7 +1830,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z14">
-        <v>8.458332000000288</v>
+        <v>8.453852694444494</v>
       </c>
       <c r="AA14">
         <v>0.066</v>
@@ -1931,7 +1931,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z15">
-        <v>8.590649999999902</v>
+        <v>8.566466276189736</v>
       </c>
       <c r="AA15">
         <v>0.05</v>
@@ -2032,7 +2032,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z16">
-        <v>8.319266000000331</v>
+        <v>8.47303437936508</v>
       </c>
       <c r="AA16">
         <v>0.046</v>
@@ -2127,7 +2127,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z17">
-        <v>8.555869999999759</v>
+        <v>8.447427389912752</v>
       </c>
       <c r="AA17">
         <v>0.16</v>
@@ -2228,7 +2228,7 @@
         <v>-4</v>
       </c>
       <c r="Z18">
-        <v>8.684945999999918</v>
+        <v>8.641522661318479</v>
       </c>
       <c r="AA18">
         <v>0.102</v>
@@ -2329,7 +2329,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z19">
-        <v>8.507029999999716</v>
+        <v>8.424627018411442</v>
       </c>
       <c r="AA19">
         <v>0.06</v>
@@ -2430,7 +2430,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z20">
-        <v>8.66001000000019</v>
+        <v>8.636608442424363</v>
       </c>
       <c r="AA20">
         <v>0.154</v>
@@ -2531,7 +2531,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z21">
-        <v>8.741863509524402</v>
+        <v>8.712416502699504</v>
       </c>
       <c r="AA21">
         <v>0.022</v>
@@ -2632,7 +2632,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z22">
-        <v>8.520710766666225</v>
+        <v>8.700157999396037</v>
       </c>
       <c r="AA22">
         <v>0.022</v>
@@ -2730,7 +2730,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z23">
-        <v>8.601016000000104</v>
+        <v>8.579560556681963</v>
       </c>
       <c r="AA23">
         <v>0.054</v>
@@ -2825,7 +2825,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z24">
-        <v>8.55453933333297</v>
+        <v>8.577874876190352</v>
       </c>
       <c r="AA24">
         <v>0.022</v>
@@ -2926,7 +2926,7 @@
         <v>-4</v>
       </c>
       <c r="Z25">
-        <v>8.472239999999626</v>
+        <v>8.589905985503107</v>
       </c>
       <c r="AA25">
         <v>0.022</v>
@@ -3027,7 +3027,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z26">
-        <v>8.618417999999677</v>
+        <v>8.590718104473112</v>
       </c>
       <c r="AA26">
         <v>0.024</v>
@@ -3128,7 +3128,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z27">
-        <v>8.532535999999826</v>
+        <v>8.454188694578024</v>
       </c>
       <c r="AA27">
         <v>0.022</v>
@@ -3229,7 +3229,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z28">
-        <v>8.430144000000725</v>
+        <v>8.378554807864584</v>
       </c>
       <c r="AA28">
         <v>0.022</v>
@@ -3330,7 +3330,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z29">
-        <v>8.674168000000035</v>
+        <v>8.493711973231816</v>
       </c>
       <c r="AA29">
         <v>0.174</v>
@@ -3428,7 +3428,7 @@
         <v>-3.8</v>
       </c>
       <c r="Z30">
-        <v>8.680532333333362</v>
+        <v>8.645422774425505</v>
       </c>
       <c r="AA30">
         <v>0.022</v>
@@ -3529,7 +3529,7 @@
         <v>-4</v>
       </c>
       <c r="Z31">
-        <v>8.676568000000113</v>
+        <v>8.645422774425505</v>
       </c>
       <c r="AA31">
         <v>0.024</v>
@@ -3630,7 +3630,7 @@
         <v>-4</v>
       </c>
       <c r="Z32">
-        <v>8.66877799999954</v>
+        <v>8.594166534343637</v>
       </c>
       <c r="AA32">
         <v>0.066</v>
@@ -3728,7 +3728,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z33">
-        <v>8.708435666666537</v>
+        <v>8.536678559465356</v>
       </c>
       <c r="AA33">
         <v>0.024</v>
@@ -3826,7 +3826,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z34">
-        <v>8.684008899999968</v>
+        <v>8.590718104473112</v>
       </c>
       <c r="AA34">
         <v>0.022</v>
@@ -3924,7 +3924,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z35">
-        <v>8.732828166667471</v>
+        <v>8.641522661318479</v>
       </c>
       <c r="AA35">
         <v>0.022</v>
@@ -4022,7 +4022,7 @@
         <v>-4</v>
       </c>
       <c r="Z36">
-        <v>8.672089999999107</v>
+        <v>8.539625559731398</v>
       </c>
       <c r="AA36">
         <v>0.036</v>
@@ -4123,7 +4123,7 @@
         <v>-4</v>
       </c>
       <c r="Z37">
-        <v>8.587893000000253</v>
+        <v>8.465131838095793</v>
       </c>
       <c r="AA37">
         <v>0.022</v>
@@ -4224,7 +4224,7 @@
         <v>-3.6</v>
       </c>
       <c r="Z38">
-        <v>8.552088666666426</v>
+        <v>8.61666977619044</v>
       </c>
       <c r="AA38">
         <v>0.022</v>
@@ -4325,7 +4325,7 @@
         <v>-3.6</v>
       </c>
       <c r="Z39">
-        <v>8.572184999999868</v>
+        <v>8.621820457143025</v>
       </c>
       <c r="AA39">
         <v>0.022</v>
@@ -4426,7 +4426,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z40">
-        <v>8.623902199999943</v>
+        <v>8.552357795072181</v>
       </c>
       <c r="AA40">
         <v>0.052</v>
@@ -4524,7 +4524,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z41">
-        <v>8.718170000000056</v>
+        <v>8.628812701801065</v>
       </c>
       <c r="AA41">
         <v>0.05</v>
@@ -4625,7 +4625,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z42">
-        <v>8.6636212333331</v>
+        <v>8.748987240683023</v>
       </c>
       <c r="AA42">
         <v>0.042</v>
@@ -4723,7 +4723,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z43">
-        <v>8.610448666666787</v>
+        <v>8.438171231313563</v>
       </c>
       <c r="AA43">
         <v>0.024</v>
@@ -4824,7 +4824,7 @@
         <v>-5</v>
       </c>
       <c r="Z44">
-        <v>8.474399999999623</v>
+        <v>8.219799669674595</v>
       </c>
       <c r="AA44">
         <v>0.022</v>
@@ -4925,7 +4925,7 @@
         <v>-5</v>
       </c>
       <c r="Z45">
-        <v>8.373543999999496</v>
+        <v>8.700157999396037</v>
       </c>
       <c r="AA45">
         <v>0.022</v>
@@ -5026,7 +5026,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z46">
-        <v>8.765635999999503</v>
+        <v>8.705104794428264</v>
       </c>
       <c r="AA46">
         <v>0.024</v>
@@ -5127,7 +5127,7 @@
         <v>-5</v>
       </c>
       <c r="Z47">
-        <v>8.746657204761766</v>
+        <v>8.6440454525251</v>
       </c>
       <c r="AA47">
         <v>0.036</v>
@@ -5228,7 +5228,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z48">
-        <v>8.752723038095047</v>
+        <v>8.6440454525251</v>
       </c>
       <c r="AA48">
         <v>0.036</v>
@@ -5329,7 +5329,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z49">
-        <v>8.744620000000149</v>
+        <v>8.700157999396037</v>
       </c>
       <c r="AA49">
         <v>0.024</v>
@@ -5430,7 +5430,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z50">
-        <v>8.690464000000187</v>
+        <v>8.719505926190017</v>
       </c>
       <c r="AA50">
         <v>0.024</v>
@@ -5531,7 +5531,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z51">
-        <v>8.791742000000388</v>
+        <v>8.808623247619151</v>
       </c>
       <c r="AA51">
         <v>0.024</v>
@@ -5626,7 +5626,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z52">
-        <v>8.602587999999978</v>
+        <v>8.68586207649007</v>
       </c>
       <c r="AA52">
         <v>0.07000000000000001</v>
@@ -5727,7 +5727,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z53">
-        <v>8.567144099999725</v>
+        <v>8.568093992309674</v>
       </c>
       <c r="AA53">
         <v>0.022</v>
@@ -5825,7 +5825,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z54">
-        <v>8.669974000000343</v>
+        <v>8.697416787088279</v>
       </c>
       <c r="AA54">
         <v>0.122</v>
@@ -5923,7 +5923,7 @@
         <v>-5</v>
       </c>
       <c r="Z55">
-        <v>8.713188799999845</v>
+        <v>8.587106575353312</v>
       </c>
       <c r="AA55">
         <v>0.024</v>
@@ -6024,7 +6024,7 @@
         <v>-5</v>
       </c>
       <c r="Z56">
-        <v>8.716191199999967</v>
+        <v>8.587106575353312</v>
       </c>
       <c r="AA56">
         <v>0.024</v>
@@ -6125,7 +6125,7 @@
         <v>-5</v>
       </c>
       <c r="Z57">
-        <v>8.732354883333622</v>
+        <v>8.644718079833094</v>
       </c>
       <c r="AA57">
         <v>0.042</v>
@@ -6226,7 +6226,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z58">
-        <v>8.539102000000154</v>
+        <v>8.604951918253549</v>
       </c>
       <c r="AA58">
         <v>0.12</v>
@@ -6327,7 +6327,7 @@
         <v>-5</v>
       </c>
       <c r="Z59">
-        <v>8.674380000000012</v>
+        <v>8.696063472926136</v>
       </c>
       <c r="AA59">
         <v>0.068</v>
@@ -6428,7 +6428,7 @@
         <v>-5</v>
       </c>
       <c r="Z60">
-        <v>8.678152000000127</v>
+        <v>8.773141501466338</v>
       </c>
       <c r="AA60">
         <v>0.066</v>
@@ -6529,7 +6529,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z61">
-        <v>8.736667000000502</v>
+        <v>8.76952584969799</v>
       </c>
       <c r="AA61">
         <v>0.042</v>
@@ -6630,7 +6630,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z62">
-        <v>8.74621599999986</v>
+        <v>8.723993207541621</v>
       </c>
       <c r="AA62">
         <v>0.058</v>
@@ -6731,7 +6731,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z63">
-        <v>8.628583999999593</v>
+        <v>8.55073876311368</v>
       </c>
       <c r="AA63">
         <v>0.058</v>
@@ -6832,7 +6832,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z64">
-        <v>8.706673199999688</v>
+        <v>8.545408744660559</v>
       </c>
       <c r="AA64">
         <v>0.092</v>
@@ -6933,7 +6933,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z65">
-        <v>8.665167999999825</v>
+        <v>8.695633968797582</v>
       </c>
       <c r="AA65">
         <v>0.146</v>
@@ -7034,7 +7034,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z66">
-        <v>8.779263999999426</v>
+        <v>8.752405795484178</v>
       </c>
       <c r="AA66">
         <v>0.108</v>
@@ -7135,7 +7135,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z67">
-        <v>8.801451333332297</v>
+        <v>8.742821801715964</v>
       </c>
       <c r="AA67">
         <v>0.05</v>
@@ -7236,7 +7236,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z68">
-        <v>8.54313199999986</v>
+        <v>8.752405795484178</v>
       </c>
       <c r="AA68">
         <v>0.158</v>
@@ -7337,7 +7337,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z69">
-        <v>8.597607999999743</v>
+        <v>8.685872273665044</v>
       </c>
       <c r="AA69">
         <v>0.138</v>
@@ -7438,7 +7438,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z70">
-        <v>8.603489999999537</v>
+        <v>8.695633968797582</v>
       </c>
       <c r="AA70">
         <v>0.132</v>
@@ -7539,7 +7539,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z71">
-        <v>8.594330000000177</v>
+        <v>8.792493134657787</v>
       </c>
       <c r="AA71">
         <v>0.172</v>
@@ -7640,7 +7640,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z72">
-        <v>8.406555999999961</v>
+        <v>8.484262812481511</v>
       </c>
       <c r="AA72">
         <v>0.22</v>
@@ -7741,7 +7741,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z73">
-        <v>8.340508000000177</v>
+        <v>8.349614949527686</v>
       </c>
       <c r="AA73">
         <v>0.126</v>
@@ -7842,7 +7842,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z74">
-        <v>8.638820804761606</v>
+        <v>8.719626882517465</v>
       </c>
       <c r="AA74">
         <v>0.08599999999999999</v>
@@ -7943,7 +7943,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z75">
-        <v>8.634597366666421</v>
+        <v>8.748987240683023</v>
       </c>
       <c r="AA75">
         <v>0.116</v>
@@ -8044,7 +8044,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z76">
-        <v>8.604401999999862</v>
+        <v>8.587148319047962</v>
       </c>
       <c r="AA76">
         <v>0.068</v>
@@ -8145,7 +8145,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z77">
-        <v>8.618556999999992</v>
+        <v>8.720436516666281</v>
       </c>
       <c r="AA77">
         <v>0.06</v>
@@ -8246,7 +8246,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z78">
-        <v>8.715349999999454</v>
+        <v>8.827762988094234</v>
       </c>
       <c r="AA78">
         <v>0.044</v>
@@ -8344,7 +8344,7 @@
         <v>-5</v>
       </c>
       <c r="Z79">
-        <v>8.647433999999755</v>
+        <v>8.712416502699504</v>
       </c>
       <c r="AA79">
         <v>0.076</v>
@@ -8445,7 +8445,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z80">
-        <v>8.730563999999955</v>
+        <v>8.639026483278048</v>
       </c>
       <c r="AA80">
         <v>0.058</v>
@@ -8546,7 +8546,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z81">
-        <v>8.644901999999639</v>
+        <v>8.728271252508412</v>
       </c>
       <c r="AA81">
         <v>0.052</v>
@@ -8647,7 +8647,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z82">
-        <v>8.727766000000384</v>
+        <v>8.659792996623162</v>
       </c>
       <c r="AA82">
         <v>0.07000000000000001</v>
@@ -8748,7 +8748,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z83">
-        <v>8.522683999999899</v>
+        <v>8.507584594299892</v>
       </c>
       <c r="AA83">
         <v>0.168</v>
@@ -8849,7 +8849,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z84">
-        <v>8.595561999999644</v>
+        <v>8.483360668391626</v>
       </c>
       <c r="AA84">
         <v>0.17</v>
@@ -8950,7 +8950,7 @@
         <v>-4.4</v>
       </c>
       <c r="Z85">
-        <v>8.408772000000113</v>
+        <v>8.531581000754041</v>
       </c>
       <c r="AA85">
         <v>0.09</v>
@@ -9042,7 +9042,7 @@
         <v>-4.2</v>
       </c>
       <c r="Z86">
-        <v>8.685287999999778</v>
+        <v>8.664348947042161</v>
       </c>
       <c r="AB86">
         <v>120</v>
@@ -9137,7 +9137,7 @@
         <v>-5</v>
       </c>
       <c r="Z87">
-        <v>8.470499999999911</v>
+        <v>8.611096299613374</v>
       </c>
       <c r="AA87">
         <v>0.068</v>
@@ -9238,7 +9238,7 @@
         <v>-5</v>
       </c>
       <c r="Z88">
-        <v>8.709832000000418</v>
+        <v>8.763272353069173</v>
       </c>
       <c r="AA88">
         <v>0.046</v>
@@ -9339,7 +9339,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z89">
-        <v>8.652219999999893</v>
+        <v>8.712416502699504</v>
       </c>
       <c r="AA89">
         <v>0.066</v>
@@ -9440,7 +9440,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z90">
-        <v>8.455769999999671</v>
+        <v>8.513558709234699</v>
       </c>
       <c r="AA90">
         <v>0.194</v>
@@ -9541,7 +9541,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z91">
-        <v>8.686693999999822</v>
+        <v>8.587106575353312</v>
       </c>
       <c r="AA91">
         <v>0.082</v>
@@ -9639,7 +9639,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z92">
-        <v>8.622507066666305</v>
+        <v>8.639564742352196</v>
       </c>
       <c r="AA92">
         <v>0.08400000000000001</v>
@@ -9713,7 +9713,7 @@
         <v>3.48</v>
       </c>
       <c r="Z93">
-        <v>8.833727333333311</v>
+        <v>8.502828340172107</v>
       </c>
       <c r="AC93">
         <v>46</v>
@@ -9799,7 +9799,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z94">
-        <v>8.564803333333662</v>
+        <v>8.583400635714565</v>
       </c>
       <c r="AA94">
         <v>0.354</v>
@@ -9897,7 +9897,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z95">
-        <v>8.525023500000465</v>
+        <v>8.505758448412609</v>
       </c>
       <c r="AA95">
         <v>0.398</v>
@@ -9995,7 +9995,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z96">
-        <v>8.557867999999885</v>
+        <v>8.534739684127166</v>
       </c>
       <c r="AA96">
         <v>0.186</v>
@@ -10096,7 +10096,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z97">
-        <v>8.660975599999858</v>
+        <v>8.76605649358696</v>
       </c>
       <c r="AA97">
         <v>0.07199999999999999</v>
@@ -10191,7 +10191,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z98">
-        <v>8.633457999999798</v>
+        <v>8.639334809613272</v>
       </c>
       <c r="AA98">
         <v>0.04</v>
@@ -10292,7 +10292,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z99">
-        <v>8.644129999999841</v>
+        <v>8.587106575353312</v>
       </c>
       <c r="AA99">
         <v>0.07000000000000001</v>
@@ -10390,7 +10390,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z100">
-        <v>8.635050000000017</v>
+        <v>8.7430797166669</v>
       </c>
       <c r="AA100">
         <v>0.058</v>
@@ -10491,7 +10491,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z101">
-        <v>8.627565999999781</v>
+        <v>8.710969176190192</v>
       </c>
       <c r="AA101">
         <v>0.066</v>
@@ -10589,7 +10589,7 @@
         <v>-5</v>
       </c>
       <c r="Z102">
-        <v>8.63604430000006</v>
+        <v>8.685906423168385</v>
       </c>
       <c r="AA102">
         <v>0.058</v>
@@ -10690,7 +10690,7 @@
         <v>-5</v>
       </c>
       <c r="Z103">
-        <v>8.640192999999952</v>
+        <v>8.77902953622055</v>
       </c>
       <c r="AA103">
         <v>0.104</v>
@@ -10791,7 +10791,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z104">
-        <v>8.707078999999752</v>
+        <v>8.742821801715964</v>
       </c>
       <c r="AA104">
         <v>0.108</v>
@@ -10892,7 +10892,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z105">
-        <v>8.709908000000105</v>
+        <v>8.63029932091232</v>
       </c>
       <c r="AA105">
         <v>0.116</v>
@@ -10993,7 +10993,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z106">
-        <v>8.696673999999904</v>
+        <v>8.576641712162971</v>
       </c>
       <c r="AA106">
         <v>0.08</v>
@@ -11094,7 +11094,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z107">
-        <v>8.774145999999927</v>
+        <v>8.752405795484178</v>
       </c>
       <c r="AA107">
         <v>0.052</v>
@@ -11195,7 +11195,7 @@
         <v>-5</v>
       </c>
       <c r="Z108">
-        <v>8.533940000000365</v>
+        <v>8.629316562598268</v>
       </c>
       <c r="AA108">
         <v>0.184</v>
@@ -11296,7 +11296,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z109">
-        <v>8.550355999999859</v>
+        <v>8.573957837301913</v>
       </c>
       <c r="AA109">
         <v>0.122</v>
@@ -11397,7 +11397,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z110">
-        <v>8.502992000000015</v>
+        <v>8.326639348534853</v>
       </c>
       <c r="AA110">
         <v>0.116</v>
@@ -11495,7 +11495,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z111">
-        <v>8.499621999999837</v>
+        <v>8.45791604118123</v>
       </c>
       <c r="AA111">
         <v>0.08799999999999999</v>
@@ -11596,7 +11596,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z112">
-        <v>8.673529999999136</v>
+        <v>8.568093992309674</v>
       </c>
       <c r="AA112">
         <v>0.074</v>
@@ -11697,7 +11697,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z113">
-        <v>8.736549999999726</v>
+        <v>8.723993207541621</v>
       </c>
       <c r="AA113">
         <v>0.07199999999999999</v>
@@ -11798,7 +11798,7 @@
         <v>-5</v>
       </c>
       <c r="Z114">
-        <v>8.653549999999743</v>
+        <v>8.750461029076462</v>
       </c>
       <c r="AA114">
         <v>0.06</v>
@@ -11899,7 +11899,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z115">
-        <v>8.763317999999467</v>
+        <v>8.743783296341906</v>
       </c>
       <c r="AA115">
         <v>0.054</v>
@@ -11994,7 +11994,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z116">
-        <v>8.57793999999984</v>
+        <v>8.742821801715964</v>
       </c>
       <c r="AA116">
         <v>0.116</v>
@@ -12095,7 +12095,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z117">
-        <v>8.684244000000193</v>
+        <v>8.583698655103484</v>
       </c>
       <c r="AA117">
         <v>0.0056</v>
@@ -12196,7 +12196,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z118">
-        <v>8.725226000000305</v>
+        <v>8.792493134657787</v>
       </c>
       <c r="AA118">
         <v>0.008800000000000001</v>
@@ -12294,7 +12294,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z119">
-        <v>8.695622000000245</v>
+        <v>8.707333120418644</v>
       </c>
       <c r="AA119">
         <v>0.0052</v>
@@ -12395,7 +12395,7 @@
         <v>-5</v>
       </c>
       <c r="Z120">
-        <v>8.744946666666431</v>
+        <v>8.752405795484178</v>
       </c>
       <c r="AA120">
         <v>0.0076</v>
@@ -12496,7 +12496,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z121">
-        <v>8.647148666666316</v>
+        <v>8.63029932091232</v>
       </c>
       <c r="AA121">
         <v>0.0114</v>
@@ -12594,7 +12594,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z122">
-        <v>8.688900628571941</v>
+        <v>8.314952755554119</v>
       </c>
       <c r="AA122">
         <v>0.008800000000000001</v>
@@ -12695,7 +12695,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z123">
-        <v>8.658551333333476</v>
+        <v>8.689795303957485</v>
       </c>
       <c r="AA123">
         <v>0.007</v>
@@ -12796,7 +12796,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z124">
-        <v>8.678772000000226</v>
+        <v>8.587106575353312</v>
       </c>
       <c r="AA124">
         <v>0.007</v>
@@ -12897,7 +12897,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z125">
-        <v>8.442770000000207</v>
+        <v>8.519027916666728</v>
       </c>
       <c r="AA125">
         <v>0.008399999999999999</v>
@@ -12998,7 +12998,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z126">
-        <v>8.550906000000481</v>
+        <v>8.454819666667099</v>
       </c>
       <c r="AA126">
         <v>0.0066</v>
@@ -13099,7 +13099,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z127">
-        <v>8.506931999999818</v>
+        <v>8.476632000000304</v>
       </c>
       <c r="AA127">
         <v>0.005</v>
@@ -13200,7 +13200,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z128">
-        <v>8.48823800000007</v>
+        <v>8.494061999999836</v>
       </c>
       <c r="AA128">
         <v>0.0094</v>
@@ -13301,7 +13301,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z129">
-        <v>8.380916000000491</v>
+        <v>8.305606000000699</v>
       </c>
       <c r="AA129">
         <v>0.0184</v>
@@ -13399,7 +13399,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z130">
-        <v>8.459842000000503</v>
+        <v>8.477991999999777</v>
       </c>
       <c r="AA130">
         <v>0.008</v>
@@ -13500,7 +13500,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z131">
-        <v>8.52751399999992</v>
+        <v>8.530100000000067</v>
       </c>
       <c r="AA131">
         <v>0.008800000000000001</v>
@@ -13598,7 +13598,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z132">
-        <v>8.531920000000149</v>
+        <v>8.458113399999876</v>
       </c>
       <c r="AA132">
         <v>0.0072</v>
@@ -13696,7 +13696,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z133">
-        <v>8.514369999999637</v>
+        <v>8.514781733332967</v>
       </c>
       <c r="AA133">
         <v>0.0098</v>
@@ -13794,7 +13794,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z134">
-        <v>8.529737999999792</v>
+        <v>8.508379999998819</v>
       </c>
       <c r="AA134">
         <v>0.0264</v>
@@ -13889,7 +13889,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z135">
-        <v>8.487949999999922</v>
+        <v>8.503508000000069</v>
       </c>
       <c r="AA135">
         <v>0.0108</v>
@@ -13990,7 +13990,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z136">
-        <v>8.467541999999732</v>
+        <v>8.4249240000005</v>
       </c>
       <c r="AA136">
         <v>0.0114</v>
@@ -14091,7 +14091,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z137">
-        <v>8.568248000000233</v>
+        <v>8.424485999999996</v>
       </c>
       <c r="AA137">
         <v>0.0194</v>
@@ -14186,7 +14186,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z138">
-        <v>8.427919999999641</v>
+        <v>8.582879999999014</v>
       </c>
       <c r="AA138">
         <v>0.0466</v>
@@ -14284,7 +14284,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z139">
-        <v>8.470483999999958</v>
+        <v>8.547314000000387</v>
       </c>
       <c r="AA139">
         <v>0.0434</v>
@@ -14382,7 +14382,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z140">
-        <v>8.466944000000112</v>
+        <v>8.611603999999977</v>
       </c>
       <c r="AA140">
         <v>0.0436</v>
@@ -14480,7 +14480,7 @@
         <v>-5</v>
       </c>
       <c r="Z141">
-        <v>8.446289999999564</v>
+        <v>8.478779999999652</v>
       </c>
       <c r="AA141">
         <v>0.0468</v>
@@ -14581,7 +14581,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z142">
-        <v>8.44518000000029</v>
+        <v>8.488584142856972</v>
       </c>
       <c r="AA142">
         <v>0.0454</v>
@@ -14682,7 +14682,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z143">
-        <v>8.491031999999908</v>
+        <v>8.475583269408855</v>
       </c>
       <c r="AA143">
         <v>0.052</v>
@@ -14783,7 +14783,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z144">
-        <v>8.45964600000009</v>
+        <v>8.543813999999513</v>
       </c>
       <c r="AA144">
         <v>0.0572</v>
@@ -14884,7 +14884,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z145">
-        <v>8.487739999999976</v>
+        <v>8.474831676190439</v>
       </c>
       <c r="AA145">
         <v>0.0374</v>
@@ -14982,7 +14982,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z146">
-        <v>8.416108000000145</v>
+        <v>8.464604000000168</v>
       </c>
       <c r="AA146">
         <v>0.0322</v>
@@ -15083,7 +15083,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z147">
-        <v>8.428906000000149</v>
+        <v>8.459944000000245</v>
       </c>
       <c r="AA147">
         <v>0.033</v>
@@ -15184,7 +15184,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z148">
-        <v>8.392246000000098</v>
+        <v>8.467886000000243</v>
       </c>
       <c r="AA148">
         <v>0.0332</v>
@@ -15285,7 +15285,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z149">
-        <v>8.593565999999933</v>
+        <v>8.604903999999118</v>
       </c>
       <c r="AA149">
         <v>0.0364</v>
@@ -15383,7 +15383,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z150">
-        <v>8.55860599999958</v>
+        <v>8.558964956349682</v>
       </c>
       <c r="AA150">
         <v>0.0444</v>
@@ -15484,7 +15484,7 @@
         <v>-6</v>
       </c>
       <c r="Z151">
-        <v>8.566342000000253</v>
+        <v>8.442144666666572</v>
       </c>
       <c r="AA151">
         <v>0.0414</v>
@@ -15585,7 +15585,7 @@
         <v>-6</v>
       </c>
       <c r="Z152">
-        <v>8.586360000000433</v>
+        <v>8.426476000000539</v>
       </c>
       <c r="AA152">
         <v>0.0414</v>
@@ -15686,7 +15686,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z153">
-        <v>8.457208000000238</v>
+        <v>8.538679333333635</v>
       </c>
       <c r="AA153">
         <v>0.0372</v>
@@ -15787,7 +15787,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z154">
-        <v>8.428226000000238</v>
+        <v>8.468658000000175</v>
       </c>
       <c r="AA154">
         <v>0.034</v>
@@ -15888,7 +15888,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z155">
-        <v>8.674611999999192</v>
+        <v>8.574817999999507</v>
       </c>
       <c r="AA155">
         <v>0.0328</v>
@@ -15989,7 +15989,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z156">
-        <v>8.462286000000361</v>
+        <v>8.449558000000435</v>
       </c>
       <c r="AA156">
         <v>0.0336</v>
@@ -16090,7 +16090,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z157">
-        <v>8.432010000000529</v>
+        <v>8.45657600000045</v>
       </c>
       <c r="AA157">
         <v>0.0324</v>
@@ -16191,7 +16191,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z158">
-        <v>8.420196000000315</v>
+        <v>8.37211200000027</v>
       </c>
       <c r="AA158">
         <v>0.0368</v>
@@ -16292,7 +16292,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z159">
-        <v>8.504277999999777</v>
+        <v>8.485569999999932</v>
       </c>
       <c r="AA159">
         <v>0.0294</v>
@@ -16393,7 +16393,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z160">
-        <v>8.575651999999785</v>
+        <v>8.543701999999934</v>
       </c>
       <c r="AA160">
         <v>0.0304</v>
@@ -16494,7 +16494,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z161">
-        <v>8.472810000000241</v>
+        <v>8.532339999999984</v>
       </c>
       <c r="AA161">
         <v>0.0444</v>
@@ -16592,7 +16592,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z162">
-        <v>8.554213999999915</v>
+        <v>8.517666166667441</v>
       </c>
       <c r="AA162">
         <v>0.0384</v>
@@ -16690,7 +16690,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z163">
-        <v>8.659810000000656</v>
+        <v>8.661251999999083</v>
       </c>
       <c r="AA163">
         <v>0.0306</v>
@@ -16791,7 +16791,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z164">
-        <v>8.520809999999706</v>
+        <v>8.436361342856634</v>
       </c>
       <c r="AA164">
         <v>0.0344</v>
@@ -16892,7 +16892,7 @@
         <v>-5</v>
       </c>
       <c r="Z165">
-        <v>8.660759999999888</v>
+        <v>8.6482654999995</v>
       </c>
       <c r="AA165">
         <v>0.0332</v>
@@ -16993,7 +16993,7 @@
         <v>-5</v>
       </c>
       <c r="Z166">
-        <v>8.681867999999138</v>
+        <v>8.650057666665909</v>
       </c>
       <c r="AA166">
         <v>0.0334</v>
@@ -17091,7 +17091,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z167">
-        <v>8.655412000000151</v>
+        <v>8.641776438094114</v>
       </c>
       <c r="AA167">
         <v>0.0312</v>
@@ -17192,7 +17192,7 @@
         <v>-5</v>
       </c>
       <c r="Z168">
-        <v>8.390286000000176</v>
+        <v>8.491125000000084</v>
       </c>
       <c r="AA168">
         <v>0.03</v>
@@ -17293,7 +17293,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z169">
-        <v>8.725930000000524</v>
+        <v>8.75717999999962</v>
       </c>
       <c r="AA169">
         <v>0.028</v>
@@ -17394,7 +17394,7 @@
         <v>-6</v>
       </c>
       <c r="Z170">
-        <v>8.714394000000684</v>
+        <v>8.76382399999992</v>
       </c>
       <c r="AA170">
         <v>0.029</v>
@@ -17495,7 +17495,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z171">
-        <v>8.710136000000148</v>
+        <v>8.769874000000346</v>
       </c>
       <c r="AA171">
         <v>0.038</v>
@@ -17593,7 +17593,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z172">
-        <v>8.41152000000019</v>
+        <v>8.484501342280227</v>
       </c>
       <c r="AA172">
         <v>0.057</v>
@@ -17691,7 +17691,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z173">
-        <v>8.397706000000262</v>
+        <v>8.558964956349682</v>
       </c>
       <c r="AA173">
         <v>0.0352</v>
@@ -17792,7 +17792,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z174">
-        <v>8.377057999999954</v>
+        <v>8.492759266665791</v>
       </c>
       <c r="AA174">
         <v>0.0292</v>
@@ -17893,7 +17893,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z175">
-        <v>8.399563999999943</v>
+        <v>8.376286857142789</v>
       </c>
       <c r="AA175">
         <v>0.038</v>
@@ -17994,7 +17994,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z176">
-        <v>8.411293999999348</v>
+        <v>8.617396333332357</v>
       </c>
       <c r="AA176">
         <v>0.038</v>
@@ -18095,7 +18095,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z177">
-        <v>8.520345999999671</v>
+        <v>8.41975599999992</v>
       </c>
       <c r="AA177">
         <v>0.033</v>
@@ -18196,7 +18196,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z178">
-        <v>8.389963999999816</v>
+        <v>8.40643959999991</v>
       </c>
       <c r="AA178">
         <v>0.0346</v>
@@ -18297,7 +18297,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z179">
-        <v>8.414003999999935</v>
+        <v>8.344387400000818</v>
       </c>
       <c r="AA179">
         <v>0.0338</v>
@@ -18395,7 +18395,7 @@
         <v>-5</v>
       </c>
       <c r="Z180">
-        <v>8.37718600000035</v>
+        <v>8.377356666666795</v>
       </c>
       <c r="AA180">
         <v>0.0306</v>
@@ -18496,7 +18496,7 @@
         <v>-5</v>
       </c>
       <c r="Z181">
-        <v>8.468577999999837</v>
+        <v>8.529016000000475</v>
       </c>
       <c r="AA181">
         <v>0.0336</v>
@@ -18597,7 +18597,7 @@
         <v>-5</v>
       </c>
       <c r="Z182">
-        <v>8.437342000000381</v>
+        <v>8.461697766667308</v>
       </c>
       <c r="AA182">
         <v>0.0452</v>
@@ -18698,7 +18698,7 @@
         <v>-5</v>
       </c>
       <c r="Z183">
-        <v>8.597978000000552</v>
+        <v>8.488226000000513</v>
       </c>
       <c r="AA183">
         <v>0.0318</v>
@@ -18799,7 +18799,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z184">
-        <v>8.514095999999737</v>
+        <v>8.493126383333358</v>
       </c>
       <c r="AA184">
         <v>0.0316</v>
@@ -18900,7 +18900,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z185">
-        <v>8.520236000000173</v>
+        <v>8.487137999999826</v>
       </c>
       <c r="AA185">
         <v>0.0396</v>
@@ -18998,7 +18998,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z186">
-        <v>8.515431999999803</v>
+        <v>8.4955673428569</v>
       </c>
       <c r="AA186">
         <v>0.0308</v>
@@ -19099,7 +19099,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z187">
-        <v>8.314016000000164</v>
+        <v>8.384132514285707</v>
       </c>
       <c r="AA187">
         <v>0.03</v>
@@ -19200,7 +19200,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z188">
-        <v>8.330712000000027</v>
+        <v>8.398488000000096</v>
       </c>
       <c r="AA188">
         <v>0.0358</v>
@@ -19301,7 +19301,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z189">
-        <v>8.476080000000188</v>
+        <v>8.434285714285672</v>
       </c>
       <c r="AA189">
         <v>0.0556</v>
@@ -19402,7 +19402,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z190">
-        <v>8.461359999999704</v>
+        <v>8.449227999999627</v>
       </c>
       <c r="AA190">
         <v>0.0382</v>
@@ -19503,7 +19503,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z191">
-        <v>8.394101999999869</v>
+        <v>8.413273999999621</v>
       </c>
       <c r="AA191">
         <v>0.0368</v>
@@ -19604,7 +19604,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z192">
-        <v>8.35578799999994</v>
+        <v>8.4185700000001</v>
       </c>
       <c r="AA192">
         <v>0.0412</v>
@@ -19705,7 +19705,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z193">
-        <v>8.479827999999756</v>
+        <v>8.398746000000052</v>
       </c>
       <c r="AA193">
         <v>0.0318</v>
@@ -19806,7 +19806,7 @@
         <v>-5</v>
       </c>
       <c r="Z194">
-        <v>8.517300000000484</v>
+        <v>8.503522000000061</v>
       </c>
       <c r="AA194">
         <v>0.0476</v>
@@ -19904,7 +19904,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z195">
-        <v>8.472671999999895</v>
+        <v>8.442241499999472</v>
       </c>
       <c r="AA195">
         <v>0.0504</v>
@@ -20005,7 +20005,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z196">
-        <v>8.499209999999962</v>
+        <v>8.508377999999777</v>
       </c>
       <c r="AA196">
         <v>0.0332</v>
@@ -20106,7 +20106,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z197">
-        <v>8.287253999999615</v>
+        <v>8.257483399999719</v>
       </c>
       <c r="AA197">
         <v>0.0326</v>
@@ -20207,7 +20207,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z198">
-        <v>8.276492000000284</v>
+        <v>8.256220000000807</v>
       </c>
       <c r="AA198">
         <v>0.0342</v>
@@ -20308,7 +20308,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z199">
-        <v>8.281640000000172</v>
+        <v>8.378676000000144</v>
       </c>
       <c r="AA199">
         <v>0.0338</v>
@@ -20409,7 +20409,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z200">
-        <v>8.245387999999693</v>
+        <v>8.321899199999956</v>
       </c>
       <c r="AA200">
         <v>0.0434</v>
@@ -20510,7 +20510,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z201">
-        <v>8.358632000000039</v>
+        <v>8.500279999999433</v>
       </c>
       <c r="AA201">
         <v>0.0428</v>
@@ -20611,7 +20611,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z202">
-        <v>8.481567999999982</v>
+        <v>8.453486000000343</v>
       </c>
       <c r="AA202">
         <v>0.053</v>
@@ -20712,7 +20712,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z203">
-        <v>8.418685999999662</v>
+        <v>8.521865999999696</v>
       </c>
       <c r="AA203">
         <v>0.04</v>
@@ -20810,7 +20810,7 @@
         <v>-6</v>
       </c>
       <c r="Z204">
-        <v>8.388258000000292</v>
+        <v>8.444725333333745</v>
       </c>
       <c r="AA204">
         <v>0.0536</v>
@@ -20911,7 +20911,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z205">
-        <v>8.403337999999644</v>
+        <v>8.429327399999137</v>
       </c>
       <c r="AA205">
         <v>0.0304</v>
@@ -21012,7 +21012,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z206">
-        <v>8.373963999999921</v>
+        <v>8.375559023809529</v>
       </c>
       <c r="AA206">
         <v>0.0306</v>
@@ -21113,7 +21113,7 @@
         <v>-6.4</v>
       </c>
       <c r="Z207">
-        <v>8.532161999999763</v>
+        <v>8.528163999999599</v>
       </c>
       <c r="AA207">
         <v>0.0312</v>
@@ -21214,7 +21214,7 @@
         <v>-6.4</v>
       </c>
       <c r="Z208">
-        <v>8.534165999999598</v>
+        <v>8.515783999999806</v>
       </c>
       <c r="AA208">
         <v>0.0322</v>
@@ -21312,7 +21312,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z209">
-        <v>8.394660000000176</v>
+        <v>8.4243066666674</v>
       </c>
       <c r="AA209">
         <v>0.0484</v>
@@ -21413,7 +21413,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z210">
-        <v>8.342841999999855</v>
+        <v>8.424090000000122</v>
       </c>
       <c r="AA210">
         <v>0.0486</v>
@@ -21514,7 +21514,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z211">
-        <v>8.430820000000022</v>
+        <v>8.605794000000216</v>
       </c>
       <c r="AA211">
         <v>0.0348</v>
@@ -21615,7 +21615,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z212">
-        <v>8.285209999999797</v>
+        <v>8.371087314285525</v>
       </c>
       <c r="AA212">
         <v>0.046</v>
@@ -21716,7 +21716,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z213">
-        <v>8.379688000000051</v>
+        <v>8.37553921428527</v>
       </c>
       <c r="AA213">
         <v>0.0358</v>
@@ -21817,7 +21817,7 @@
         <v>-6</v>
       </c>
       <c r="Z214">
-        <v>8.434889999999843</v>
+        <v>8.459645333333071</v>
       </c>
       <c r="AA214">
         <v>0.0326</v>
@@ -21918,7 +21918,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z215">
-        <v>8.51008800000009</v>
+        <v>8.417210000000036</v>
       </c>
       <c r="AA215">
         <v>0.0158</v>
@@ -22019,7 +22019,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z216">
-        <v>8.52531200000023</v>
+        <v>8.530028000000137</v>
       </c>
       <c r="AA216">
         <v>0.0114</v>
@@ -22120,7 +22120,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z217">
-        <v>8.512048000000096</v>
+        <v>8.52861000000007</v>
       </c>
       <c r="AA217">
         <v>0.03</v>
@@ -22221,7 +22221,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z218">
-        <v>8.489571999999672</v>
+        <v>8.500107099999745</v>
       </c>
       <c r="AA218">
         <v>0.0026</v>
@@ -22322,7 +22322,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z219">
-        <v>8.466501999999748</v>
+        <v>8.324635999999563</v>
       </c>
       <c r="AA219">
         <v>0.0048</v>
@@ -22423,7 +22423,7 @@
         <v>-5</v>
       </c>
       <c r="Z220">
-        <v>8.546440000000134</v>
+        <v>8.531086000000169</v>
       </c>
       <c r="AA220">
         <v>0.008999999999999999</v>
@@ -22524,7 +22524,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z221">
-        <v>8.469478000000709</v>
+        <v>8.473532000000764</v>
       </c>
       <c r="AA221">
         <v>0.0094</v>
@@ -22625,7 +22625,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z222">
-        <v>8.457413999999881</v>
+        <v>8.403209800000175</v>
       </c>
       <c r="AA222">
         <v>0.0026</v>
@@ -22726,7 +22726,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z223">
-        <v>8.429735999999702</v>
+        <v>8.459899911110435</v>
       </c>
       <c r="AA223">
         <v>0.0026</v>
@@ -22827,7 +22827,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z224">
-        <v>8.430275999999514</v>
+        <v>8.46821466666716</v>
       </c>
       <c r="AA224">
         <v>0.0026</v>
@@ -22928,7 +22928,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z225">
-        <v>8.419941999999912</v>
+        <v>8.538270000001008</v>
       </c>
       <c r="AA225">
         <v>0.0026</v>
@@ -23029,7 +23029,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z226">
-        <v>8.577620000000234</v>
+        <v>8.625308000000572</v>
       </c>
       <c r="AA226">
         <v>0.0154</v>
@@ -23130,7 +23130,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z227">
-        <v>8.491848000000099</v>
+        <v>8.472357999999831</v>
       </c>
       <c r="AA227">
         <v>0.0066</v>
@@ -23225,7 +23225,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z228">
-        <v>8.448680000000046</v>
+        <v>8.448956333332697</v>
       </c>
       <c r="AA228">
         <v>0.0036</v>
@@ -23326,7 +23326,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z229">
-        <v>8.497869999999967</v>
+        <v>8.454737500000196</v>
       </c>
       <c r="AA229">
         <v>0.0048</v>
@@ -23427,7 +23427,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z230">
-        <v>8.414856000000217</v>
+        <v>8.394784500000043</v>
       </c>
       <c r="AA230">
         <v>0.0026</v>
@@ -23528,7 +23528,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z231">
-        <v>8.406685999999215</v>
+        <v>8.442566066665927</v>
       </c>
       <c r="AA231">
         <v>0.0026</v>
@@ -23629,7 +23629,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z232">
-        <v>8.408417999999829</v>
+        <v>8.291642566666869</v>
       </c>
       <c r="AA232">
         <v>0.0026</v>
@@ -23727,7 +23727,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z233">
-        <v>8.488983999999478</v>
+        <v>8.412917299999645</v>
       </c>
       <c r="AA233">
         <v>0.0196</v>
@@ -23828,7 +23828,7 @@
         <v>-5</v>
       </c>
       <c r="Z234">
-        <v>8.417743999999729</v>
+        <v>8.462347357142029</v>
       </c>
       <c r="AA234">
         <v>0.023</v>
@@ -23929,7 +23929,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z235">
-        <v>8.584618000000477</v>
+        <v>8.544998000000493</v>
       </c>
       <c r="AA235">
         <v>0.0218</v>
@@ -24030,7 +24030,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z236">
-        <v>8.60056000000059</v>
+        <v>8.636570000001242</v>
       </c>
       <c r="AA236">
         <v>0.0282</v>
@@ -24131,7 +24131,7 @@
         <v>-5</v>
       </c>
       <c r="Z237">
-        <v>8.47033600000014</v>
+        <v>8.484063544444595</v>
       </c>
       <c r="AA237">
         <v>0.0166</v>
@@ -24232,7 +24232,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z238">
-        <v>8.533484000000453</v>
+        <v>8.476502000001046</v>
       </c>
       <c r="AA238">
         <v>0.0162</v>
@@ -24333,7 +24333,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z239">
-        <v>8.591884000000434</v>
+        <v>8.462174218254157</v>
       </c>
       <c r="AA239">
         <v>0.0126</v>
@@ -24434,7 +24434,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z240">
-        <v>8.443919999999695</v>
+        <v>8.316218000000982</v>
       </c>
       <c r="AA240">
         <v>0.0102</v>
@@ -24535,7 +24535,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z241">
-        <v>8.480171999999826</v>
+        <v>8.576512000000459</v>
       </c>
       <c r="AA241">
         <v>0.0108</v>
@@ -24636,7 +24636,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z242">
-        <v>8.479595999999919</v>
+        <v>8.371508000000288</v>
       </c>
       <c r="AA242">
         <v>0.0124</v>
@@ -24737,7 +24737,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z243">
-        <v>8.568528000000054</v>
+        <v>8.623832000000309</v>
       </c>
       <c r="AA243">
         <v>0.009599999999999999</v>
@@ -24835,7 +24835,7 @@
         <v>-5.4</v>
       </c>
       <c r="Z244">
-        <v>8.454812000000013</v>
+        <v>8.562327333333123</v>
       </c>
       <c r="AA244">
         <v>0.0292</v>
@@ -24936,7 +24936,7 @@
         <v>-5</v>
       </c>
       <c r="Z245">
-        <v>8.535477999999742</v>
+        <v>8.459664000000027</v>
       </c>
       <c r="AA245">
         <v>0.0118</v>
@@ -25037,7 +25037,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z246">
-        <v>8.368535999999787</v>
+        <v>8.41294446666689</v>
       </c>
       <c r="AA246">
         <v>0.0042</v>
@@ -25138,7 +25138,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z247">
-        <v>8.393677999999866</v>
+        <v>8.411862000000449</v>
       </c>
       <c r="AA247">
         <v>0.0062</v>
@@ -25239,7 +25239,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z248">
-        <v>8.377746000000094</v>
+        <v>8.353888000000259</v>
       </c>
       <c r="AA248">
         <v>0.0024</v>
@@ -25340,7 +25340,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z249">
-        <v>8.537150000000128</v>
+        <v>8.581017999999903</v>
       </c>
       <c r="AA249">
         <v>0.0024</v>
@@ -25435,7 +25435,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z250">
-        <v>8.550521999999987</v>
+        <v>8.641133999999193</v>
       </c>
       <c r="AA250">
         <v>0.0026</v>
@@ -25536,7 +25536,7 @@
         <v>-6</v>
       </c>
       <c r="Z251">
-        <v>8.444302000000345</v>
+        <v>8.50107640000026</v>
       </c>
       <c r="AA251">
         <v>0.0026</v>
@@ -25634,7 +25634,7 @@
         <v>-5</v>
       </c>
       <c r="Z252">
-        <v>8.411497999999993</v>
+        <v>8.560347999999646</v>
       </c>
       <c r="AA252">
         <v>0.0026</v>
@@ -25735,7 +25735,7 @@
         <v>-5</v>
       </c>
       <c r="Z253">
-        <v>8.428590000000471</v>
+        <v>8.446178000000499</v>
       </c>
       <c r="AA253">
         <v>0.006</v>
@@ -25830,7 +25830,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z254">
-        <v>8.477415999999961</v>
+        <v>8.452274142857572</v>
       </c>
       <c r="AA254">
         <v>0.0196</v>
@@ -25931,7 +25931,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z255">
-        <v>8.524825999999964</v>
+        <v>8.574180000000124</v>
       </c>
       <c r="AA255">
         <v>0.0476</v>
@@ -26032,7 +26032,7 @@
         <v>-4.8</v>
       </c>
       <c r="Z256">
-        <v>8.584823999999925</v>
+        <v>8.562287999999819</v>
       </c>
       <c r="AA256">
         <v>0.0136</v>
@@ -26118,7 +26118,7 @@
         <v>-4.6</v>
       </c>
       <c r="Z257">
-        <v>8.437287999999972</v>
+        <v>8.35106399999988</v>
       </c>
       <c r="AA257">
         <v>0.011</v>
@@ -26213,7 +26213,7 @@
         <v>-5.2</v>
       </c>
       <c r="Z258">
-        <v>8.371726000000081</v>
+        <v>8.361714000000518</v>
       </c>
       <c r="AA258">
         <v>0.0282</v>
@@ -26314,7 +26314,7 @@
         <v>-6</v>
       </c>
       <c r="Z259">
-        <v>8.662592000000288</v>
+        <v>8.644877999999796</v>
       </c>
       <c r="AA259">
         <v>0.0148</v>
@@ -26415,7 +26415,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z260">
-        <v>8.503938000000241</v>
+        <v>8.533016000000602</v>
       </c>
       <c r="AA260">
         <v>0.0108</v>
@@ -26516,7 +26516,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z261">
-        <v>8.472302000000274</v>
+        <v>8.505002000000195</v>
       </c>
       <c r="AA261">
         <v>0.0026</v>
@@ -26617,7 +26617,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z262">
-        <v>8.574681999999751</v>
+        <v>8.577874000000238</v>
       </c>
       <c r="AA262">
         <v>0.0026</v>
@@ -26718,7 +26718,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z263">
-        <v>8.52501400000034</v>
+        <v>8.50264599999962</v>
       </c>
       <c r="AA263">
         <v>0.0074</v>
@@ -26819,7 +26819,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z264">
-        <v>8.403457999999961</v>
+        <v>8.436242399999374</v>
       </c>
       <c r="AA264">
         <v>0.0038</v>
@@ -26920,7 +26920,7 @@
         <v>-5.6</v>
       </c>
       <c r="Z265">
-        <v>8.600633999999379</v>
+        <v>8.638385999999597</v>
       </c>
       <c r="AA265">
         <v>0.0024</v>
@@ -27021,7 +27021,7 @@
         <v>-6.2</v>
       </c>
       <c r="Z266">
-        <v>8.387948000000158</v>
+        <v>8.430285400000622</v>
       </c>
       <c r="AA266">
         <v>0.0068</v>
@@ -27122,7 +27122,7 @@
         <v>-6</v>
       </c>
       <c r="Z267">
-        <v>8.347581999999951</v>
+        <v>8.436238000000081</v>
       </c>
       <c r="AA267">
         <v>0.0026</v>
@@ -27223,7 +27223,7 @@
         <v>-5.8</v>
       </c>
       <c r="Z268">
-        <v>8.21922800000114</v>
+        <v>8.160782000001266</v>
       </c>
       <c r="AA268">
         <v>0.0062</v>

</xml_diff>